<commit_message>
1. Optimize repairing ticket by ajax 2. Update abnormal report while updating monitor journal
</commit_message>
<xml_diff>
--- a/report_template/monitorJournal.xlsx
+++ b/report_template/monitorJournal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -38,9 +38,6 @@
     <t>例行性維護保養工作內容</t>
   </si>
   <si>
-    <t>異常檢修排除工作內容</t>
-  </si>
-  <si>
     <t>環境變遷及事件紀錄</t>
   </si>
   <si>
@@ -73,13 +70,17 @@
   </si>
   <si>
     <t>備註</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>異常原因及故障檢修工作內容</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -276,14 +277,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,54 +301,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -357,6 +340,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -364,6 +356,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,6 +469,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -503,6 +521,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,7 +717,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -691,49 +726,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
@@ -745,218 +780,218 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="18"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="18"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="19"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="20"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="20"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="20"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="32"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
+      <c r="A23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E24" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
@@ -964,18 +999,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H22"/>
+    <mergeCell ref="A6:H10"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H22"/>
-    <mergeCell ref="A6:H10"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="E24:H24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>